<commit_message>
Latest data, fix small bug with listing of sources on single ind. page
</commit_message>
<xml_diff>
--- a/datastatic/datasets/online/SDG6_Fresh_Water_withdrawal_WB_2014.xlsx
+++ b/datastatic/datasets/online/SDG6_Fresh_Water_withdrawal_WB_2014.xlsx
@@ -17,15 +17,15 @@
     <t>Country Name</t>
   </si>
   <si>
+    <t>sponsor</t>
+  </si>
+  <si>
     <t>2011</t>
   </si>
   <si>
     <t>2012</t>
   </si>
   <si>
-    <t>sponsor</t>
-  </si>
-  <si>
     <t>2013</t>
   </si>
   <si>
@@ -56,21 +56,21 @@
     <t>Chile</t>
   </si>
   <si>
+    <t>original_title</t>
+  </si>
+  <si>
     <t>China</t>
   </si>
   <si>
+    <t>Freshwater withdrawals</t>
+  </si>
+  <si>
     <t>Croatia</t>
   </si>
   <si>
-    <t>original_title</t>
-  </si>
-  <si>
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Freshwater withdrawals</t>
-  </si>
-  <si>
     <t>Czech Republic</t>
   </si>
   <si>
@@ -80,19 +80,22 @@
     <t>Estonia</t>
   </si>
   <si>
+    <t>original_indicator_code</t>
+  </si>
+  <si>
     <t>Finland</t>
   </si>
   <si>
+    <t>ER.H2O.FWTL.K3</t>
+  </si>
+  <si>
     <t>France</t>
   </si>
   <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>original_indicator_code</t>
-  </si>
-  <si>
-    <t>ER.H2O.FWTL.K3</t>
+    <t>title_German</t>
   </si>
   <si>
     <t>Greece</t>
@@ -104,7 +107,7 @@
     <t>Iceland</t>
   </si>
   <si>
-    <t>title_German</t>
+    <t>Frischwasserverbrauch</t>
   </si>
   <si>
     <t>India</t>
@@ -116,7 +119,7 @@
     <t>Israel</t>
   </si>
   <si>
-    <t>Frischwasserverbrauch</t>
+    <t>sdg</t>
   </si>
   <si>
     <t>Italy</t>
@@ -128,18 +131,24 @@
     <t>Kosovo</t>
   </si>
   <si>
-    <t>sdg</t>
-  </si>
-  <si>
     <t>Latvia</t>
   </si>
   <si>
+    <t>short_indicator_description</t>
+  </si>
+  <si>
     <t>Lithuania</t>
   </si>
   <si>
     <t>Luxembourg</t>
   </si>
   <si>
+    <t>short_indicator_description$de</t>
+  </si>
+  <si>
+    <t>Jährlicher Frischwasserverbrauch pro Kopf</t>
+  </si>
+  <si>
     <t>Macedonia, FYR</t>
   </si>
   <si>
@@ -149,81 +158,84 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>short_indicator_description</t>
+    <t>short_indicator_description$en</t>
   </si>
   <si>
     <t>Montenegro</t>
   </si>
   <si>
+    <t>Annual freshwater withdrawal per capita</t>
+  </si>
+  <si>
     <t>Netherlands</t>
   </si>
   <si>
     <t>New Zealand</t>
   </si>
   <si>
-    <t>short_indicator_description$de</t>
+    <t>long_indicator_description</t>
   </si>
   <si>
     <t>Norway</t>
   </si>
   <si>
-    <t>Jährlicher Frischwasserverbrauch pro Kopf</t>
-  </si>
-  <si>
     <t>Poland</t>
   </si>
   <si>
+    <t>long_indicator_description$de$text</t>
+  </si>
+  <si>
     <t>Portugal</t>
   </si>
   <si>
     <t>Romania</t>
   </si>
   <si>
-    <t>short_indicator_description$en</t>
-  </si>
-  <si>
-    <t>Annual freshwater withdrawal per capita</t>
+    <t xml:space="preserve">In SDG Unterziel 6.4 wird angestrebt, die Effizienz von Frischwasserverbrauch zu erhöhen, um Mangel zu vermeiden und Frischwasser für die gesamte Weltbevölkerung zugänglich zu machen. Jährlicher Frischwasserverbrauch ist der Wasserverbrauch in Kubikmeter pro Kopf für landwirtschaftlichen, industriellen und privaten Verbrauch (Verdunstungen in Wasserbecken bleiben ungezählt). Der Verbrauch beinhaltet auch Wasser von Entsalzungsanlagen in Ländern wo diese eine wesentliche Wasserquelle sind. Weltweit wird extrem viel Frischwasser in der Landwirtschaft verbraucht, sodass dies ein wichtiger Bereich ist, in dem die Wassereffizienz erhöht werden muss. </t>
   </si>
   <si>
     <t>Russia</t>
   </si>
   <si>
-    <t>long_indicator_description</t>
+    <t>long_indicator_description$de$baseunit</t>
+  </si>
+  <si>
+    <t>m3 / Kopf</t>
+  </si>
+  <si>
+    <t>long_indicator_description$en$text</t>
   </si>
   <si>
     <t>Serbia</t>
   </si>
   <si>
-    <t>long_indicator_description$de$text</t>
-  </si>
-  <si>
     <t>Slovak Republic</t>
   </si>
   <si>
+    <t xml:space="preserve">According to SDG target 6.4, the efficiency of freshwater use needs to be increased in order to reduce water scarcity and ensure freshwater access for all. Annual freshwater withdrawals refer to total water withdrawals in cubic meter per capita, combining industrial, agricultural and private use, but not counting evaporation losses from storage basins. Withdrawals also include water from desalination plants in countries where they are a significant source. Much of the freshwater worldwide is used for agriculture, so reducing freshwater use in this area is particularly important.  </t>
+  </si>
+  <si>
     <t>Slovenia</t>
   </si>
   <si>
-    <t xml:space="preserve">In SDG Unterziel 6.4 wird angestrebt, die Effizienz von Frischwasserverbrauch zu erhöhen, um Mangel zu vermeiden und Frischwasser für die gesamte Weltbevölkerung zugänglich zu machen. Jährlicher Frischwasserverbrauch ist der Wasserverbrauch in Kubikmeter pro Kopf für landwirtschaftlichen, industriellen und privaten Verbrauch (Verdunstungen in Wasserbecken bleiben ungezählt). Der Verbrauch beinhaltet auch Wasser von Entsalzungsanlagen in Ländern wo diese eine wesentliche Wasserquelle sind. Weltweit wird extrem viel Frischwasser in der Landwirtschaft verbraucht, sodass dies ein wichtiger Bereich ist, in dem die Wassereffizienz erhöht werden muss. </t>
-  </si>
-  <si>
     <t>South Africa</t>
   </si>
   <si>
     <t>South Korea</t>
   </si>
   <si>
+    <t>long_indicator_description$en$baseunit</t>
+  </si>
+  <si>
+    <t>m3 / capita</t>
+  </si>
+  <si>
     <t>Spain</t>
   </si>
   <si>
-    <t>long_indicator_description$de$baseunit</t>
-  </si>
-  <si>
     <t>Sweden</t>
   </si>
   <si>
-    <t>m3 / Kopf</t>
-  </si>
-  <si>
     <t>Switzerland</t>
   </si>
   <si>
@@ -233,19 +245,7 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>long_indicator_description$en$text</t>
-  </si>
-  <si>
     <t>United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">According to SDG target 6.4, the efficiency of freshwater use needs to be increased in order to reduce water scarcity and ensure freshwater access for all. Annual freshwater withdrawals refer to total water withdrawals in cubic meter per capita, combining industrial, agricultural and private use, but not counting evaporation losses from storage basins. Withdrawals also include water from desalination plants in countries where they are a significant source. Much of the freshwater worldwide is used for agriculture, so reducing freshwater use in this area is particularly important.  </t>
-  </si>
-  <si>
-    <t>long_indicator_description$en$baseunit</t>
-  </si>
-  <si>
-    <t>m3 / capita</t>
   </si>
   <si>
     <t>target</t>
@@ -718,7 +718,7 @@
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="2"/>
@@ -755,10 +755,10 @@
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -794,10 +794,10 @@
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -833,10 +833,10 @@
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -872,7 +872,7 @@
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="7">
         <v>6.0</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
@@ -948,10 +948,10 @@
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -987,10 +987,10 @@
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -1063,10 +1063,10 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1102,10 +1102,10 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1141,10 +1141,10 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="A55" s="23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B55" s="30">
         <v>149.5379494</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="A57" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B57" s="30">
         <v>221.296086</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="62" ht="13.5" customHeight="1">
       <c r="A62" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B62" s="30">
         <v>1201.498779</v>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="A63" s="23" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B63" s="30">
         <v>454.6142216</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="65" ht="13.5" customHeight="1">
       <c r="A65" s="23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B65" s="30">
         <v>407.9893804</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="A67" s="23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B67" s="30">
         <v>884.1016219</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="A71" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B71" s="30">
         <v>511.9359836</v>
@@ -2552,7 +2552,7 @@
     </row>
     <row r="72" ht="13.5" customHeight="1">
       <c r="A72" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B72" s="30">
         <v>9197.094561</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="A73" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B73" s="30">
         <v>163.9512911</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="75" ht="13.5" customHeight="1">
       <c r="A75" s="23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B75" s="30">
         <v>237.8373115</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="76" ht="13.5" customHeight="1">
       <c r="A76" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B76" s="30">
         <v>884.2039878</v>
@@ -2612,7 +2612,7 @@
     </row>
     <row r="77" ht="13.5" customHeight="1">
       <c r="A77" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B77" s="30">
         <v>640.6736945</v>
@@ -2624,7 +2624,7 @@
     </row>
     <row r="78" ht="13.5" customHeight="1">
       <c r="A78" s="23" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B78" s="30">
         <v>579.0898393</v>
@@ -2672,7 +2672,7 @@
     </row>
     <row r="82" ht="13.5" customHeight="1">
       <c r="A82" s="23" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B82" s="30">
         <v>215.3209336</v>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="83" ht="13.5" customHeight="1">
       <c r="A83" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B83" s="30">
         <v>77.47353587</v>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="85" ht="13.5" customHeight="1">
       <c r="A85" s="23" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B85" s="30">
         <v>105.9986335</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="88" ht="13.5" customHeight="1">
       <c r="A88" s="23" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B88" s="30">
         <v>635.6356309</v>
@@ -2768,7 +2768,7 @@
     </row>
     <row r="90" ht="13.5" customHeight="1">
       <c r="A90" s="23" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B90" s="26">
         <v>1153.291793</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="92" ht="13.5" customHeight="1">
       <c r="A92" s="23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B92" s="26">
         <v>589.0331603</v>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="94" ht="13.5" customHeight="1">
       <c r="A94" s="23" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B94" s="26">
         <v>302.0119971</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="95" ht="13.5" customHeight="1">
       <c r="A95" s="23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B95" s="26">
         <v>879.8140036</v>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="104" ht="13.5" customHeight="1">
       <c r="A104" s="23" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B104" s="26">
         <v>560.6261942</v>
@@ -2948,7 +2948,7 @@
     </row>
     <row r="105" ht="13.5" customHeight="1">
       <c r="A105" s="23" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B105" s="26">
         <v>803.5561804</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="108" ht="13.5" customHeight="1">
       <c r="A108" s="23" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B108" s="26">
         <v>277.3277118</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="109" ht="13.5" customHeight="1">
       <c r="A109" s="23" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B109" s="26">
         <v>244.8511348</v>
@@ -7350,10 +7350,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -7500,7 +7500,7 @@
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3">
         <v>1.34413E9</v>
@@ -7517,7 +7517,7 @@
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3">
         <v>4280622.0</v>
@@ -7534,7 +7534,7 @@
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3">
         <v>1116644.0</v>
@@ -7602,7 +7602,7 @@
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3">
         <v>5388272.0</v>
@@ -7619,7 +7619,7 @@
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3">
         <v>6.5342776E7</v>
@@ -7636,7 +7636,7 @@
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3">
         <v>8.1797673E7</v>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3">
         <v>1.1123213E7</v>
@@ -7670,7 +7670,7 @@
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3">
         <v>9971727.0</v>
@@ -7687,7 +7687,7 @@
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3">
         <v>319014.0</v>
@@ -7704,7 +7704,7 @@
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3">
         <v>1.247446011E9</v>
@@ -7721,7 +7721,7 @@
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3">
         <v>4576794.0</v>
@@ -7738,7 +7738,7 @@
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3">
         <v>7765800.0</v>
@@ -7755,7 +7755,7 @@
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3">
         <v>5.9379449E7</v>
@@ -7772,7 +7772,7 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3">
         <v>1.27817277E8</v>
@@ -7789,7 +7789,7 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3">
         <v>1790957.0</v>
@@ -7823,7 +7823,7 @@
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="3">
         <v>3028115.0</v>
@@ -7840,7 +7840,7 @@
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3">
         <v>518347.0</v>
@@ -7857,7 +7857,7 @@
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3">
         <v>2065888.0</v>
@@ -7874,7 +7874,7 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B32" s="3">
         <v>416268.0</v>
@@ -7891,7 +7891,7 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B33" s="3">
         <v>1.20365271E8</v>
@@ -7908,7 +7908,7 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B34" s="3">
         <v>620079.0</v>
@@ -7925,7 +7925,7 @@
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B35" s="3">
         <v>1.6693074E7</v>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3">
         <v>4384000.0</v>
@@ -7959,7 +7959,7 @@
     </row>
     <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B37" s="3">
         <v>4953088.0</v>
@@ -7976,7 +7976,7 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B38" s="3">
         <v>3.8063255E7</v>
@@ -7993,7 +7993,7 @@
     </row>
     <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B39" s="3">
         <v>1.055756E7</v>
@@ -8010,7 +8010,7 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B40" s="3">
         <v>2.0147528E7</v>
@@ -8027,7 +8027,7 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B41" s="3">
         <v>1.42960868E8</v>
@@ -8044,7 +8044,7 @@
     </row>
     <row r="42" ht="13.5" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B42" s="3">
         <v>7234099.0</v>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B43" s="3">
         <v>5398384.0</v>
@@ -8078,7 +8078,7 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B44" s="3">
         <v>2052843.0</v>
@@ -8095,7 +8095,7 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B45" s="3">
         <v>5.1553479E7</v>
@@ -8112,7 +8112,7 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B46" s="3">
         <v>4.977944E7</v>
@@ -8129,7 +8129,7 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B47" s="3">
         <v>4.6742697E7</v>
@@ -8146,7 +8146,7 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B48" s="3">
         <v>9449213.0</v>
@@ -8163,7 +8163,7 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B49" s="3">
         <v>7912398.0</v>
@@ -8180,7 +8180,7 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B50" s="3">
         <v>7.3199372E7</v>
@@ -8197,7 +8197,7 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B51" s="3">
         <v>6.3258918E7</v>
@@ -8214,7 +8214,7 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B52" s="3">
         <v>3.11721632E8</v>

</xml_diff>